<commit_message>
Completado de Secciones de los siguientes documentos:
-Plan de Pruebas.
-Arquitectura del Sistema.
-Plan de SQA.
-Propuesta de Desarrollo.

Actualización del Seguimiento de la Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -468,40 +468,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -815,47 +815,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="16" t="s">
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="20" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="20"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="20"/>
+      <c r="A4" s="23"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
@@ -865,11 +865,11 @@
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="16"/>
+      <c r="G4" s="20"/>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -893,7 +893,7 @@
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="15"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
@@ -915,7 +915,7 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
@@ -937,7 +937,7 @@
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
@@ -959,7 +959,7 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="15"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -981,7 +981,7 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="15"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="15"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
@@ -1025,7 +1025,7 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="15"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="15"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1059,7 +1059,7 @@
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1083,7 +1083,7 @@
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="15"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1105,7 +1105,7 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="15"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
@@ -1127,7 +1127,7 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="15"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="15"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="8" t="s">
         <v>78</v>
       </c>
@@ -1161,7 +1161,7 @@
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="15"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="8" t="s">
         <v>22</v>
       </c>
@@ -1173,7 +1173,7 @@
       <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="15"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
@@ -1185,7 +1185,7 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="15"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
@@ -1197,7 +1197,7 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="15"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
@@ -1219,7 +1219,7 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="15"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="9" t="s">
         <v>26</v>
       </c>
@@ -1241,7 +1241,7 @@
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="15"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="9" t="s">
         <v>27</v>
       </c>
@@ -1263,7 +1263,7 @@
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="15"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="8" t="s">
         <v>28</v>
       </c>
@@ -1275,7 +1275,7 @@
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="15"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
@@ -1287,7 +1287,7 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="15"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="9" t="s">
         <v>30</v>
       </c>
@@ -1299,7 +1299,7 @@
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="15"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="9" t="s">
         <v>31</v>
       </c>
@@ -1311,7 +1311,7 @@
       <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="15"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="9" t="s">
         <v>32</v>
       </c>
@@ -1323,7 +1323,7 @@
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="15"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="7" t="s">
         <v>33</v>
       </c>
@@ -1345,7 +1345,7 @@
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="15"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="7" t="s">
         <v>34</v>
       </c>
@@ -1367,7 +1367,7 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="15"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="8" t="s">
         <v>35</v>
       </c>
@@ -1389,7 +1389,7 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="15"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="7" t="s">
         <v>36</v>
       </c>
@@ -1411,7 +1411,7 @@
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -1425,7 +1425,7 @@
       <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="15"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="8" t="s">
         <v>39</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="15"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="8" t="s">
         <v>40</v>
       </c>
@@ -1449,7 +1449,7 @@
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="8" t="s">
@@ -1463,7 +1463,7 @@
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="24"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="7" t="s">
         <v>43</v>
       </c>
@@ -1481,7 +1481,7 @@
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="25"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="7" t="s">
         <v>44</v>
       </c>
@@ -1509,10 +1509,10 @@
         <v>77</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>64</v>
@@ -1523,7 +1523,7 @@
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="15" t="s">
+      <c r="A41" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -1547,7 +1547,7 @@
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="15"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="8" t="s">
         <v>49</v>
       </c>
@@ -1559,7 +1559,7 @@
       <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="15"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="8" t="s">
         <v>50</v>
       </c>
@@ -1571,7 +1571,7 @@
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="15"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="7" t="s">
         <v>51</v>
       </c>
@@ -1593,7 +1593,7 @@
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="15" t="s">
+      <c r="A45" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B45" s="8" t="s">
@@ -1617,7 +1617,7 @@
       <c r="H45" s="13"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="15"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="9" t="s">
         <v>54</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="H46" s="13"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="15"/>
+      <c r="A47" s="16"/>
       <c r="B47" s="8" t="s">
         <v>55</v>
       </c>
@@ -1707,18 +1707,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Completado de los siguientes documentos:
-Plan de Pruebas.
-Plan de Iteración 4 - Elaboración.
-Plan de Iteración 4 - Construcción.

Actualización del Documento: Seguimiento de Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -469,9 +469,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -480,27 +501,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -815,15 +815,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
@@ -833,29 +833,29 @@
       <c r="N1" s="15"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="20" t="s">
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="18" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="23"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="23"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
@@ -865,11 +865,11 @@
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -893,7 +893,7 @@
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
@@ -915,7 +915,7 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
@@ -937,7 +937,7 @@
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="16"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
@@ -959,7 +959,7 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="16"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -981,7 +981,7 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="16"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
@@ -1003,7 +1003,7 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="16"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
@@ -1025,7 +1025,7 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="16"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="16"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1059,7 +1059,7 @@
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1083,7 +1083,7 @@
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="16"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1105,7 +1105,7 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="16"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
@@ -1127,7 +1127,7 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="16"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="16"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="8" t="s">
         <v>78</v>
       </c>
@@ -1161,7 +1161,7 @@
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="16"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="8" t="s">
         <v>22</v>
       </c>
@@ -1173,7 +1173,7 @@
       <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="16"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
@@ -1185,7 +1185,7 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="16"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
@@ -1197,7 +1197,7 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="16"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
@@ -1219,7 +1219,7 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="16"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="9" t="s">
         <v>26</v>
       </c>
@@ -1241,7 +1241,7 @@
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="16"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="9" t="s">
         <v>27</v>
       </c>
@@ -1263,7 +1263,7 @@
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="16"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="8" t="s">
         <v>28</v>
       </c>
@@ -1275,7 +1275,7 @@
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="16"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
@@ -1287,7 +1287,7 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="16"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="9" t="s">
         <v>30</v>
       </c>
@@ -1299,7 +1299,7 @@
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="16"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="9" t="s">
         <v>31</v>
       </c>
@@ -1311,7 +1311,7 @@
       <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="16"/>
+      <c r="A29" s="17"/>
       <c r="B29" s="9" t="s">
         <v>32</v>
       </c>
@@ -1323,7 +1323,7 @@
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="16"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="7" t="s">
         <v>33</v>
       </c>
@@ -1345,7 +1345,7 @@
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="16"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="7" t="s">
         <v>34</v>
       </c>
@@ -1367,7 +1367,7 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="16"/>
+      <c r="A32" s="17"/>
       <c r="B32" s="8" t="s">
         <v>35</v>
       </c>
@@ -1389,7 +1389,7 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="16"/>
+      <c r="A33" s="17"/>
       <c r="B33" s="7" t="s">
         <v>36</v>
       </c>
@@ -1411,7 +1411,7 @@
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -1425,7 +1425,7 @@
       <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="16"/>
+      <c r="A35" s="17"/>
       <c r="B35" s="8" t="s">
         <v>39</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="16"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="8" t="s">
         <v>40</v>
       </c>
@@ -1449,7 +1449,7 @@
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="24" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="8" t="s">
@@ -1463,7 +1463,7 @@
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="18"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="7" t="s">
         <v>43</v>
       </c>
@@ -1481,7 +1481,7 @@
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="19"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="7" t="s">
         <v>44</v>
       </c>
@@ -1523,7 +1523,7 @@
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -1547,7 +1547,7 @@
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="16"/>
+      <c r="A42" s="17"/>
       <c r="B42" s="8" t="s">
         <v>49</v>
       </c>
@@ -1559,7 +1559,7 @@
       <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="16"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="8" t="s">
         <v>50</v>
       </c>
@@ -1571,7 +1571,7 @@
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="16"/>
+      <c r="A44" s="17"/>
       <c r="B44" s="7" t="s">
         <v>51</v>
       </c>
@@ -1579,10 +1579,10 @@
         <v>70</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>64</v>
@@ -1593,7 +1593,7 @@
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B45" s="8" t="s">
@@ -1617,7 +1617,7 @@
       <c r="H45" s="13"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="16"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="9" t="s">
         <v>54</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="H46" s="13"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="16"/>
+      <c r="A47" s="17"/>
       <c r="B47" s="8" t="s">
         <v>55</v>
       </c>
@@ -1707,6 +1707,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A47"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1714,11 +1719,6 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
-Actualización del Diagrama de CU del Sistema VASPA.
-Creación de diagramas de Casos de Uso individuales del sistema.

-Creación y actualización de los siguientes documentos:
Especificación CU Generar Informe Gerencial y Especificación CU Realizar Carga Masiva de Programas.

-Completado y actualización de los siguientes documentos:
Especificación de Requerimientos y Modelo de Casos de Uso.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -901,10 +901,10 @@
         <v>70</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>64</v>
@@ -1625,10 +1625,10 @@
         <v>70</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
-Creación y agregado del documento: Resumen de Reunion.
-Actualización y completado de secciones de los siguientes documentos:

Arquitectura del Sistema, Modelo de Diseño y Seguimiento Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -469,12 +469,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -491,15 +500,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -798,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -815,15 +815,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
@@ -833,29 +833,29 @@
       <c r="N1" s="15"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18" t="s">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="21" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="21"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="21"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
@@ -865,11 +865,11 @@
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="18"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -893,7 +893,7 @@
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="17"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
@@ -915,7 +915,7 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="17"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
@@ -937,7 +937,7 @@
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="17"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
@@ -959,7 +959,7 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="17"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -981,7 +981,7 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="17"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
@@ -992,10 +992,10 @@
         <v>64</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>73</v>
@@ -1003,7 +1003,7 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="17"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
@@ -1025,7 +1025,7 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="17"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="17"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1059,7 +1059,7 @@
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1083,7 +1083,7 @@
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="17"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1105,7 +1105,7 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="17"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
@@ -1127,7 +1127,7 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="17"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="17"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="8" t="s">
         <v>78</v>
       </c>
@@ -1161,7 +1161,7 @@
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="17"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="8" t="s">
         <v>22</v>
       </c>
@@ -1173,7 +1173,7 @@
       <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="17"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
@@ -1185,7 +1185,7 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="17"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
@@ -1197,7 +1197,7 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="17"/>
+      <c r="A22" s="16"/>
       <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
@@ -1219,7 +1219,7 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="17"/>
+      <c r="A23" s="16"/>
       <c r="B23" s="9" t="s">
         <v>26</v>
       </c>
@@ -1241,7 +1241,7 @@
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="17"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="9" t="s">
         <v>27</v>
       </c>
@@ -1263,7 +1263,7 @@
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="17"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="8" t="s">
         <v>28</v>
       </c>
@@ -1275,7 +1275,7 @@
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="17"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
@@ -1287,7 +1287,7 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="17"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="9" t="s">
         <v>30</v>
       </c>
@@ -1299,7 +1299,7 @@
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="17"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="9" t="s">
         <v>31</v>
       </c>
@@ -1311,7 +1311,7 @@
       <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="17"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="9" t="s">
         <v>32</v>
       </c>
@@ -1323,7 +1323,7 @@
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="17"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="7" t="s">
         <v>33</v>
       </c>
@@ -1345,7 +1345,7 @@
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="17"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="7" t="s">
         <v>34</v>
       </c>
@@ -1367,7 +1367,7 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="17"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="8" t="s">
         <v>35</v>
       </c>
@@ -1389,7 +1389,7 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="17"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="7" t="s">
         <v>36</v>
       </c>
@@ -1411,7 +1411,7 @@
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="16" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -1425,7 +1425,7 @@
       <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="17"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="8" t="s">
         <v>39</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="17"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="8" t="s">
         <v>40</v>
       </c>
@@ -1449,7 +1449,7 @@
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="8" t="s">
@@ -1463,7 +1463,7 @@
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="25"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="7" t="s">
         <v>43</v>
       </c>
@@ -1481,7 +1481,7 @@
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="26"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="7" t="s">
         <v>44</v>
       </c>
@@ -1523,7 +1523,7 @@
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -1547,7 +1547,7 @@
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="17"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="8" t="s">
         <v>49</v>
       </c>
@@ -1559,7 +1559,7 @@
       <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="17"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="8" t="s">
         <v>50</v>
       </c>
@@ -1571,7 +1571,7 @@
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="17"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="7" t="s">
         <v>51</v>
       </c>
@@ -1593,7 +1593,7 @@
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>52</v>
       </c>
       <c r="B45" s="8" t="s">
@@ -1617,7 +1617,7 @@
       <c r="H45" s="13"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="17"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="9" t="s">
         <v>54</v>
       </c>
@@ -1639,7 +1639,7 @@
       <c r="H46" s="13"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="17"/>
+      <c r="A47" s="16"/>
       <c r="B47" s="8" t="s">
         <v>55</v>
       </c>
@@ -1707,11 +1707,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A47"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1719,6 +1714,11 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Actualización y completado de los siguientes documentos:
-Arquitectura del Sistema.
-Modelo de Datos.
-Modelo de Diseño.
-Seguimiento Documentacion.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="84">
   <si>
     <t>DOCUMENTACIÓN - METODOLOGÍA DE DESARROLLO PSI</t>
   </si>
@@ -469,9 +469,30 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -479,27 +500,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -799,7 +799,7 @@
   <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -815,15 +815,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
@@ -833,29 +833,29 @@
       <c r="N1" s="15"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="21" t="s">
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="18" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="24"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="21"/>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
@@ -865,11 +865,11 @@
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="21"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="17" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -893,7 +893,7 @@
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
@@ -915,7 +915,7 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
@@ -937,7 +937,7 @@
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="16"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
@@ -945,10 +945,10 @@
         <v>70</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>64</v>
@@ -959,7 +959,7 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="16"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -967,10 +967,10 @@
         <v>70</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>64</v>
@@ -981,7 +981,7 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="16"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
@@ -989,10 +989,10 @@
         <v>70</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>64</v>
@@ -1003,7 +1003,7 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="16"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
@@ -1025,7 +1025,7 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="16"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="16"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1059,7 +1059,7 @@
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1083,7 +1083,7 @@
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="16"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1105,7 +1105,7 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="16"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
@@ -1127,7 +1127,7 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="16"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
@@ -1139,7 +1139,7 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="16"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="8" t="s">
         <v>78</v>
       </c>
@@ -1161,7 +1161,7 @@
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="16"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="8" t="s">
         <v>22</v>
       </c>
@@ -1173,7 +1173,7 @@
       <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="16"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
@@ -1185,7 +1185,7 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="16"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
@@ -1197,7 +1197,7 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="16"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
@@ -1219,7 +1219,7 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="16"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="9" t="s">
         <v>26</v>
       </c>
@@ -1241,7 +1241,7 @@
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="16"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="9" t="s">
         <v>27</v>
       </c>
@@ -1263,7 +1263,7 @@
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="16"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="8" t="s">
         <v>28</v>
       </c>
@@ -1275,7 +1275,7 @@
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="16"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
@@ -1287,7 +1287,7 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="16"/>
+      <c r="A27" s="17"/>
       <c r="B27" s="9" t="s">
         <v>30</v>
       </c>
@@ -1299,7 +1299,7 @@
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="16"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="9" t="s">
         <v>31</v>
       </c>
@@ -1311,7 +1311,7 @@
       <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="16"/>
+      <c r="A29" s="17"/>
       <c r="B29" s="9" t="s">
         <v>32</v>
       </c>
@@ -1323,7 +1323,7 @@
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="16"/>
+      <c r="A30" s="17"/>
       <c r="B30" s="7" t="s">
         <v>33</v>
       </c>
@@ -1345,7 +1345,7 @@
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="16"/>
+      <c r="A31" s="17"/>
       <c r="B31" s="7" t="s">
         <v>34</v>
       </c>
@@ -1367,7 +1367,7 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="16"/>
+      <c r="A32" s="17"/>
       <c r="B32" s="8" t="s">
         <v>35</v>
       </c>
@@ -1389,7 +1389,7 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="16"/>
+      <c r="A33" s="17"/>
       <c r="B33" s="7" t="s">
         <v>36</v>
       </c>
@@ -1411,7 +1411,7 @@
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -1425,7 +1425,7 @@
       <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="16"/>
+      <c r="A35" s="17"/>
       <c r="B35" s="8" t="s">
         <v>39</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="16"/>
+      <c r="A36" s="17"/>
       <c r="B36" s="8" t="s">
         <v>40</v>
       </c>
@@ -1449,21 +1449,29 @@
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="24" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
+      <c r="C37" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="G37" s="12"/>
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="18"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="7" t="s">
         <v>43</v>
       </c>
@@ -1481,7 +1489,7 @@
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="19"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="7" t="s">
         <v>44</v>
       </c>
@@ -1523,7 +1531,7 @@
       <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -1547,7 +1555,7 @@
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="16"/>
+      <c r="A42" s="17"/>
       <c r="B42" s="8" t="s">
         <v>49</v>
       </c>
@@ -1559,7 +1567,7 @@
       <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="16"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="8" t="s">
         <v>50</v>
       </c>
@@ -1571,7 +1579,7 @@
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="16"/>
+      <c r="A44" s="17"/>
       <c r="B44" s="7" t="s">
         <v>51</v>
       </c>
@@ -1593,7 +1601,7 @@
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="17" t="s">
         <v>52</v>
       </c>
       <c r="B45" s="8" t="s">
@@ -1617,7 +1625,7 @@
       <c r="H45" s="13"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="16"/>
+      <c r="A46" s="17"/>
       <c r="B46" s="9" t="s">
         <v>54</v>
       </c>
@@ -1639,7 +1647,7 @@
       <c r="H46" s="13"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="16"/>
+      <c r="A47" s="17"/>
       <c r="B47" s="8" t="s">
         <v>55</v>
       </c>
@@ -1707,6 +1715,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A45:A47"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1714,11 +1727,6 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
-Agregación y modificación de Screenshots de los distintos CU.
-Completado de secciones del Manual de Usuario.

-Actualización del Documento: Seguimiento Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="86">
   <si>
     <t>DOCUMENTACIÓN - METODOLOGÍA DE DESARROLLO PSI</t>
   </si>
@@ -475,21 +475,27 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -508,15 +514,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -813,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -830,15 +828,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
@@ -848,29 +846,29 @@
       <c r="N1" s="15"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="21" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="23" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="24"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
@@ -880,11 +878,11 @@
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="21"/>
+      <c r="G4" s="23"/>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="18" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -908,7 +906,7 @@
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="20"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
@@ -930,7 +928,7 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="20"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
@@ -952,7 +950,7 @@
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="20"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
@@ -974,7 +972,7 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="20"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -996,7 +994,7 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="20"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
@@ -1018,7 +1016,7 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="20"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
@@ -1040,7 +1038,7 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="20"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1062,7 +1060,7 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="20"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1074,7 +1072,7 @@
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1098,7 +1096,7 @@
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="20"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1120,7 +1118,7 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="20"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
@@ -1142,7 +1140,7 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="20"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
@@ -1154,7 +1152,7 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="20"/>
+      <c r="A18" s="18"/>
       <c r="B18" s="8" t="s">
         <v>78</v>
       </c>
@@ -1176,7 +1174,7 @@
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="20"/>
+      <c r="A19" s="18"/>
       <c r="B19" s="8" t="s">
         <v>22</v>
       </c>
@@ -1188,7 +1186,7 @@
       <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="20"/>
+      <c r="A20" s="18"/>
       <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
@@ -1200,7 +1198,7 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="20"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
@@ -1212,7 +1210,7 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="20"/>
+      <c r="A22" s="18"/>
       <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
@@ -1234,7 +1232,7 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="20"/>
+      <c r="A23" s="18"/>
       <c r="B23" s="9" t="s">
         <v>26</v>
       </c>
@@ -1256,7 +1254,7 @@
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="20"/>
+      <c r="A24" s="18"/>
       <c r="B24" s="9" t="s">
         <v>27</v>
       </c>
@@ -1278,7 +1276,7 @@
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="20"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="8" t="s">
         <v>28</v>
       </c>
@@ -1290,7 +1288,7 @@
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="20"/>
+      <c r="A26" s="18"/>
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
@@ -1302,7 +1300,7 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="20"/>
+      <c r="A27" s="18"/>
       <c r="B27" s="9" t="s">
         <v>30</v>
       </c>
@@ -1314,7 +1312,7 @@
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="20"/>
+      <c r="A28" s="18"/>
       <c r="B28" s="9" t="s">
         <v>31</v>
       </c>
@@ -1326,7 +1324,7 @@
       <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="20"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="9" t="s">
         <v>32</v>
       </c>
@@ -1338,7 +1336,7 @@
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="20"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="7" t="s">
         <v>33</v>
       </c>
@@ -1360,7 +1358,7 @@
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="20"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="7" t="s">
         <v>34</v>
       </c>
@@ -1382,7 +1380,7 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="20"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="8" t="s">
         <v>35</v>
       </c>
@@ -1404,7 +1402,7 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="20"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="7" t="s">
         <v>36</v>
       </c>
@@ -1426,7 +1424,7 @@
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="18" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -1440,7 +1438,7 @@
       <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="20"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="8" t="s">
         <v>39</v>
       </c>
@@ -1452,7 +1450,7 @@
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="20"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="8" t="s">
         <v>40</v>
       </c>
@@ -1464,33 +1462,33 @@
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="8" t="s">
-        <v>42</v>
+      <c r="B37" s="17" t="s">
+        <v>84</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D37" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G37" s="12" t="s">
+      <c r="D37" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="G37" s="6" t="s">
         <v>85</v>
       </c>
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="28"/>
-      <c r="B38" s="7" t="s">
-        <v>43</v>
+      <c r="A38" s="20"/>
+      <c r="B38" s="8" t="s">
+        <v>42</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>76</v>
@@ -1510,9 +1508,9 @@
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="29"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>76</v>
@@ -1532,69 +1530,79 @@
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="21"/>
+      <c r="B40" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B41" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C41" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G40" s="12" t="s">
+      <c r="D41" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G41" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="H40" s="13"/>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" s="20" t="s">
+      <c r="H41" s="13"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="B42" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G41" s="12" t="s">
+      <c r="D42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="H41" s="13"/>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="20"/>
-      <c r="B42" s="8" t="s">
+      <c r="H42" s="13"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="18"/>
+      <c r="B43" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="13"/>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="20"/>
-      <c r="B43" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -1604,33 +1612,21 @@
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="20"/>
-      <c r="B44" s="7" t="s">
+      <c r="A44" s="18"/>
+      <c r="B44" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="13"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="18"/>
+      <c r="B45" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G44" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="H44" s="13"/>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>53</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>70</v>
@@ -1645,14 +1641,16 @@
         <v>64</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H45" s="13"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="20"/>
-      <c r="B46" s="9" t="s">
-        <v>54</v>
+      <c r="A46" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>53</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>70</v>
@@ -1667,89 +1665,94 @@
         <v>64</v>
       </c>
       <c r="G46" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="H46" s="13"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="18"/>
+      <c r="B47" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G47" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="H46" s="13"/>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="20"/>
-      <c r="B47" s="8" t="s">
+      <c r="H47" s="13"/>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="18"/>
+      <c r="B48" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="13"/>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B48" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E48" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F48" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="13"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:8">
       <c r="A63" s="11"/>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:8">
       <c r="A64" s="11"/>
     </row>
     <row r="66" spans="1:1">
@@ -1763,11 +1766,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A37:A39"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A45:A47"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1775,6 +1773,11 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Se cambian algunos nombres de documentos, quitándoles la versión.
Se modifica el Seguimiento Documentacion.xlsx
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\00 - REPOSITORIOS\Sistema VASPA\trunk\Seguimiento del Sistema\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="87">
   <si>
     <t>DOCUMENTACIÓN - METODOLOGÍA DE DESARROLLO PSI</t>
   </si>
@@ -274,13 +279,16 @@
   </si>
   <si>
     <t>SI (/Manuales)</t>
+  </si>
+  <si>
+    <t>SI (actualizar antes de entregar)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,9 +489,31 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -493,34 +523,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -567,7 +583,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -599,9 +615,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -633,6 +650,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -808,35 +826,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
     <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="35.28515625" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="44.7109375" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
@@ -845,30 +863,30 @@
       <c r="M1" s="15"/>
       <c r="N1" s="15"/>
     </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="25" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="23" t="s">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="21" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="26"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="26"/>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
@@ -878,11 +896,11 @@
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="23"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="14"/>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -905,8 +923,8 @@
       </c>
       <c r="H5" s="13"/>
     </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="18"/>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
@@ -927,8 +945,8 @@
       </c>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="18"/>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
@@ -949,8 +967,8 @@
       </c>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="18"/>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
@@ -958,7 +976,7 @@
         <v>70</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>64</v>
@@ -971,8 +989,8 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="18"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -993,8 +1011,8 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="18"/>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
       <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
@@ -1015,8 +1033,8 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="18"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
@@ -1037,8 +1055,8 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="18"/>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
       <c r="B12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1059,8 +1077,8 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="18"/>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1071,8 +1089,8 @@
       <c r="G13" s="12"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="18" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1095,8 +1113,8 @@
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="18"/>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
       <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1117,8 +1135,8 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="18"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
       <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
@@ -1139,8 +1157,8 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="18"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
       <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
@@ -1151,8 +1169,8 @@
       <c r="G17" s="12"/>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="18"/>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
       <c r="B18" s="8" t="s">
         <v>78</v>
       </c>
@@ -1173,8 +1191,8 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="18"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
       <c r="B19" s="8" t="s">
         <v>22</v>
       </c>
@@ -1185,8 +1203,8 @@
       <c r="G19" s="12"/>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="18"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
       <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
@@ -1197,8 +1215,8 @@
       <c r="G20" s="12"/>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="18"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
@@ -1209,8 +1227,8 @@
       <c r="G21" s="12"/>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="18"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
       <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
@@ -1231,8 +1249,8 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="18"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
       <c r="B23" s="9" t="s">
         <v>26</v>
       </c>
@@ -1253,8 +1271,8 @@
       </c>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="18"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
       <c r="B24" s="9" t="s">
         <v>27</v>
       </c>
@@ -1275,8 +1293,8 @@
       </c>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="18"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
       <c r="B25" s="8" t="s">
         <v>28</v>
       </c>
@@ -1287,8 +1305,8 @@
       <c r="G25" s="12"/>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="18"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
@@ -1299,8 +1317,8 @@
       <c r="G26" s="12"/>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="1:8">
-      <c r="A27" s="18"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
       <c r="B27" s="9" t="s">
         <v>30</v>
       </c>
@@ -1311,8 +1329,8 @@
       <c r="G27" s="12"/>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="1:8">
-      <c r="A28" s="18"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
       <c r="B28" s="9" t="s">
         <v>31</v>
       </c>
@@ -1323,8 +1341,8 @@
       <c r="G28" s="12"/>
       <c r="H28" s="13"/>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="18"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
       <c r="B29" s="9" t="s">
         <v>32</v>
       </c>
@@ -1335,8 +1353,8 @@
       <c r="G29" s="12"/>
       <c r="H29" s="13"/>
     </row>
-    <row r="30" spans="1:8">
-      <c r="A30" s="18"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
       <c r="B30" s="7" t="s">
         <v>33</v>
       </c>
@@ -1357,8 +1375,8 @@
       </c>
       <c r="H30" s="13"/>
     </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="18"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
       <c r="B31" s="7" t="s">
         <v>34</v>
       </c>
@@ -1379,8 +1397,8 @@
       </c>
       <c r="H31" s="13"/>
     </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="18"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
       <c r="B32" s="8" t="s">
         <v>35</v>
       </c>
@@ -1401,8 +1419,8 @@
       </c>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="18"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
       <c r="B33" s="7" t="s">
         <v>36</v>
       </c>
@@ -1423,8 +1441,8 @@
       </c>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="18" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -1437,8 +1455,8 @@
       <c r="G34" s="12"/>
       <c r="H34" s="13"/>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="18"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
       <c r="B35" s="8" t="s">
         <v>39</v>
       </c>
@@ -1449,8 +1467,8 @@
       <c r="G35" s="12"/>
       <c r="H35" s="13"/>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="18"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="20"/>
       <c r="B36" s="8" t="s">
         <v>40</v>
       </c>
@@ -1461,8 +1479,8 @@
       <c r="G36" s="12"/>
       <c r="H36" s="13"/>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="19" t="s">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="17" t="s">
@@ -1485,8 +1503,8 @@
       </c>
       <c r="H37" s="13"/>
     </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="20"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="28"/>
       <c r="B38" s="8" t="s">
         <v>42</v>
       </c>
@@ -1507,8 +1525,8 @@
       </c>
       <c r="H38" s="13"/>
     </row>
-    <row r="39" spans="1:8">
-      <c r="A39" s="20"/>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="28"/>
       <c r="B39" s="7" t="s">
         <v>43</v>
       </c>
@@ -1529,8 +1547,8 @@
       </c>
       <c r="H39" s="13"/>
     </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="21"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="29"/>
       <c r="B40" s="7" t="s">
         <v>44</v>
       </c>
@@ -1551,7 +1569,7 @@
       </c>
       <c r="H40" s="13"/>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>45</v>
       </c>
@@ -1562,7 +1580,7 @@
         <v>77</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>64</v>
@@ -1575,8 +1593,8 @@
       </c>
       <c r="H41" s="13"/>
     </row>
-    <row r="42" spans="1:8">
-      <c r="A42" s="18" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="20" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="8" t="s">
@@ -1599,8 +1617,8 @@
       </c>
       <c r="H42" s="13"/>
     </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="18"/>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="20"/>
       <c r="B43" s="8" t="s">
         <v>49</v>
       </c>
@@ -1611,8 +1629,8 @@
       <c r="G43" s="12"/>
       <c r="H43" s="13"/>
     </row>
-    <row r="44" spans="1:8">
-      <c r="A44" s="18"/>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="20"/>
       <c r="B44" s="8" t="s">
         <v>50</v>
       </c>
@@ -1623,8 +1641,8 @@
       <c r="G44" s="12"/>
       <c r="H44" s="13"/>
     </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="18"/>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="20"/>
       <c r="B45" s="7" t="s">
         <v>51</v>
       </c>
@@ -1645,8 +1663,8 @@
       </c>
       <c r="H45" s="13"/>
     </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="18" t="s">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="20" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="8" t="s">
@@ -1669,8 +1687,8 @@
       </c>
       <c r="H46" s="13"/>
     </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="18"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="20"/>
       <c r="B47" s="9" t="s">
         <v>54</v>
       </c>
@@ -1691,8 +1709,8 @@
       </c>
       <c r="H47" s="13"/>
     </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="18"/>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="20"/>
       <c r="B48" s="8" t="s">
         <v>55</v>
       </c>
@@ -1703,69 +1721,74 @@
       <c r="G48" s="6"/>
       <c r="H48" s="13"/>
     </row>
-    <row r="49" spans="1:8">
-      <c r="G49" s="29"/>
-      <c r="H49" s="29"/>
-    </row>
-    <row r="50" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>58</v>
       </c>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="G50" s="18"/>
+      <c r="H50" s="18"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1773,11 +1796,6 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1785,24 +1803,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualización de documento de SQA Cambio de nombre a archivos con la terminación "vX.Y" Eliminación de archivos temporales
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="88">
   <si>
     <t>DOCUMENTACIÓN - METODOLOGÍA DE DESARROLLO PSI</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t>SI (actualizar antes de entregar)</t>
+  </si>
+  <si>
+    <t>SI (actualizar)</t>
   </si>
 </sst>
 </file>
@@ -490,12 +493,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -512,15 +524,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -829,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -846,15 +849,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
@@ -864,29 +867,29 @@
       <c r="N1" s="15"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="21" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="24" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="24"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="24"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
@@ -896,11 +899,11 @@
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="21"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -924,7 +927,7 @@
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
@@ -946,7 +949,7 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
@@ -968,7 +971,7 @@
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
@@ -990,7 +993,7 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -998,7 +1001,7 @@
         <v>70</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>64</v>
@@ -1012,7 +1015,7 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
@@ -1034,7 +1037,7 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
@@ -1056,7 +1059,7 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1078,7 +1081,7 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1090,7 +1093,7 @@
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1114,7 +1117,7 @@
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1136,7 +1139,7 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
@@ -1158,7 +1161,7 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
@@ -1170,7 +1173,7 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="8" t="s">
         <v>78</v>
       </c>
@@ -1192,7 +1195,7 @@
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="8" t="s">
         <v>22</v>
       </c>
@@ -1204,7 +1207,7 @@
       <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
@@ -1216,7 +1219,7 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
@@ -1228,7 +1231,7 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
@@ -1250,7 +1253,7 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="9" t="s">
         <v>26</v>
       </c>
@@ -1272,7 +1275,7 @@
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="20"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="9" t="s">
         <v>27</v>
       </c>
@@ -1294,7 +1297,7 @@
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="20"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="8" t="s">
         <v>28</v>
       </c>
@@ -1306,7 +1309,7 @@
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
@@ -1318,7 +1321,7 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="9" t="s">
         <v>30</v>
       </c>
@@ -1330,7 +1333,7 @@
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="9" t="s">
         <v>31</v>
       </c>
@@ -1342,7 +1345,7 @@
       <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="9" t="s">
         <v>32</v>
       </c>
@@ -1354,7 +1357,7 @@
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="7" t="s">
         <v>33</v>
       </c>
@@ -1376,7 +1379,7 @@
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="7" t="s">
         <v>34</v>
       </c>
@@ -1398,7 +1401,7 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="8" t="s">
         <v>35</v>
       </c>
@@ -1420,7 +1423,7 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="7" t="s">
         <v>36</v>
       </c>
@@ -1442,7 +1445,7 @@
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="20" t="s">
+      <c r="A34" s="19" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -1456,7 +1459,7 @@
       <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="8" t="s">
         <v>39</v>
       </c>
@@ -1468,7 +1471,7 @@
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="8" t="s">
         <v>40</v>
       </c>
@@ -1480,7 +1483,7 @@
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="27" t="s">
+      <c r="A37" s="20" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="17" t="s">
@@ -1504,7 +1507,7 @@
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="28"/>
+      <c r="A38" s="21"/>
       <c r="B38" s="8" t="s">
         <v>42</v>
       </c>
@@ -1526,7 +1529,7 @@
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="28"/>
+      <c r="A39" s="21"/>
       <c r="B39" s="7" t="s">
         <v>43</v>
       </c>
@@ -1548,7 +1551,7 @@
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="29"/>
+      <c r="A40" s="22"/>
       <c r="B40" s="7" t="s">
         <v>44</v>
       </c>
@@ -1594,7 +1597,7 @@
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="19" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="8" t="s">
@@ -1618,7 +1621,7 @@
       <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="8" t="s">
         <v>49</v>
       </c>
@@ -1630,7 +1633,7 @@
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="8" t="s">
         <v>50</v>
       </c>
@@ -1642,7 +1645,7 @@
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="7" t="s">
         <v>51</v>
       </c>
@@ -1664,7 +1667,7 @@
       <c r="H45" s="13"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
+      <c r="A46" s="19" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="8" t="s">
@@ -1688,7 +1691,7 @@
       <c r="H46" s="13"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="9" t="s">
         <v>54</v>
       </c>
@@ -1710,7 +1713,7 @@
       <c r="H47" s="13"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="8" t="s">
         <v>55</v>
       </c>
@@ -1784,11 +1787,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1796,6 +1794,11 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalización del Plan de SQA.docx Actualización de Memoria del Proyecto.docx Actualización de Seguimiento Documentacion.xlsx
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -16,12 +16,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="89">
   <si>
     <t>DOCUMENTACIÓN - METODOLOGÍA DE DESARROLLO PSI</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>SI (actualizar)</t>
+  </si>
+  <si>
+    <t>Francisco Estrada y Fabricio González</t>
   </si>
 </sst>
 </file>
@@ -493,9 +496,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -503,27 +527,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -832,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,15 +852,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
@@ -867,29 +870,29 @@
       <c r="N1" s="15"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="24" t="s">
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="21" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
@@ -899,11 +902,11 @@
       <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="14"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -927,7 +930,7 @@
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
@@ -949,7 +952,7 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
@@ -971,7 +974,7 @@
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
@@ -993,7 +996,7 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
@@ -1015,7 +1018,7 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="7" t="s">
         <v>14</v>
       </c>
@@ -1037,7 +1040,7 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
@@ -1059,7 +1062,7 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="7" t="s">
         <v>79</v>
       </c>
@@ -1081,7 +1084,7 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1093,7 +1096,7 @@
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="20" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -1117,7 +1120,7 @@
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
@@ -1139,7 +1142,7 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="8" t="s">
         <v>20</v>
       </c>
@@ -1161,7 +1164,7 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="8" t="s">
         <v>21</v>
       </c>
@@ -1173,7 +1176,7 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="8" t="s">
         <v>78</v>
       </c>
@@ -1195,7 +1198,7 @@
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="8" t="s">
         <v>22</v>
       </c>
@@ -1207,7 +1210,7 @@
       <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
@@ -1219,7 +1222,7 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
@@ -1231,7 +1234,7 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="7" t="s">
         <v>25</v>
       </c>
@@ -1253,7 +1256,7 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="9" t="s">
         <v>26</v>
       </c>
@@ -1275,7 +1278,7 @@
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="9" t="s">
         <v>27</v>
       </c>
@@ -1297,7 +1300,7 @@
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
+      <c r="A25" s="20"/>
       <c r="B25" s="8" t="s">
         <v>28</v>
       </c>
@@ -1309,7 +1312,7 @@
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="8" t="s">
         <v>29</v>
       </c>
@@ -1321,7 +1324,7 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
+      <c r="A27" s="20"/>
       <c r="B27" s="9" t="s">
         <v>30</v>
       </c>
@@ -1333,7 +1336,7 @@
       <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="9" t="s">
         <v>31</v>
       </c>
@@ -1345,7 +1348,7 @@
       <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
+      <c r="A29" s="20"/>
       <c r="B29" s="9" t="s">
         <v>32</v>
       </c>
@@ -1357,19 +1360,17 @@
       <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="19"/>
+      <c r="A30" s="20"/>
       <c r="B30" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>65</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E30" s="6"/>
       <c r="F30" s="6" t="s">
         <v>64</v>
       </c>
@@ -1379,7 +1380,7 @@
       <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="19"/>
+      <c r="A31" s="20"/>
       <c r="B31" s="7" t="s">
         <v>34</v>
       </c>
@@ -1401,7 +1402,7 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
+      <c r="A32" s="20"/>
       <c r="B32" s="8" t="s">
         <v>35</v>
       </c>
@@ -1423,7 +1424,7 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="19"/>
+      <c r="A33" s="20"/>
       <c r="B33" s="7" t="s">
         <v>36</v>
       </c>
@@ -1445,7 +1446,7 @@
       <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="20" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="8" t="s">
@@ -1459,7 +1460,7 @@
       <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="19"/>
+      <c r="A35" s="20"/>
       <c r="B35" s="8" t="s">
         <v>39</v>
       </c>
@@ -1471,7 +1472,7 @@
       <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="8" t="s">
         <v>40</v>
       </c>
@@ -1483,7 +1484,7 @@
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
+      <c r="A37" s="27" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="17" t="s">
@@ -1507,7 +1508,7 @@
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="8" t="s">
         <v>42</v>
       </c>
@@ -1529,7 +1530,7 @@
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="7" t="s">
         <v>43</v>
       </c>
@@ -1551,7 +1552,7 @@
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
+      <c r="A40" s="29"/>
       <c r="B40" s="7" t="s">
         <v>44</v>
       </c>
@@ -1597,7 +1598,7 @@
       <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="20" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="8" t="s">
@@ -1621,7 +1622,7 @@
       <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="8" t="s">
         <v>49</v>
       </c>
@@ -1633,7 +1634,7 @@
       <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
+      <c r="A44" s="20"/>
       <c r="B44" s="8" t="s">
         <v>50</v>
       </c>
@@ -1645,7 +1646,7 @@
       <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
+      <c r="A45" s="20"/>
       <c r="B45" s="7" t="s">
         <v>51</v>
       </c>
@@ -1667,7 +1668,7 @@
       <c r="H45" s="13"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="20" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="8" t="s">
@@ -1691,7 +1692,7 @@
       <c r="H46" s="13"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
+      <c r="A47" s="20"/>
       <c r="B47" s="9" t="s">
         <v>54</v>
       </c>
@@ -1713,7 +1714,7 @@
       <c r="H47" s="13"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
+      <c r="A48" s="20"/>
       <c r="B48" s="8" t="s">
         <v>55</v>
       </c>
@@ -1787,6 +1788,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1794,11 +1800,6 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
-Actualización y finalización del documento de Especificación del CU Ingresar al Sistema.
-Elaboración del diagrama de secuencia del CU Ingresar al Sistema.

-Actualización del documento: Seguimiento Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -288,9 +288,6 @@
     <t>DOCUMENTACIÓN - ESPECIFICACIONES DE CU</t>
   </si>
   <si>
-    <t>En total se encuentran finalizados 17 de 21 Documentos de Especificación.</t>
-  </si>
-  <si>
     <t>Caso de Uso</t>
   </si>
   <si>
@@ -358,6 +355,9 @@
   </si>
   <si>
     <t>Ver Vigencia de Programas</t>
+  </si>
+  <si>
+    <t>En total se encuentran finalizados 18 de 21 Documentos de Especificación.</t>
   </si>
 </sst>
 </file>
@@ -581,12 +581,21 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -603,15 +612,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -950,15 +950,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -968,29 +968,29 @@
       <c r="N1" s="12"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="24" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="27" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="27"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
@@ -1000,11 +1000,11 @@
       <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1028,7 +1028,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="23"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="23"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1072,7 +1072,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="23"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1094,7 +1094,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="23"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1116,7 +1116,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="23"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1138,7 +1138,7 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="23"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1160,7 +1160,7 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="23"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1182,7 +1182,7 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="23"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1218,7 +1218,7 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="23"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="23"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1262,7 +1262,7 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="23"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="23"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1296,7 +1296,7 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="23"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="23"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1320,7 +1320,7 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="23"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1332,7 +1332,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="23"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="23"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="23"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="23"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1410,7 +1410,7 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="23"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="23"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1434,7 +1434,7 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="23"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="23"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="23"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1480,7 +1480,7 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="23"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1502,7 +1502,7 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="23"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
@@ -1524,7 +1524,7 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="23"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1546,7 +1546,7 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1560,7 +1560,7 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="23"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1572,7 +1572,7 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="23"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1584,7 +1584,7 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="23" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1608,7 +1608,7 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="31"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1630,7 +1630,7 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="31"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
@@ -1652,7 +1652,7 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="32"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1698,7 +1698,7 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1722,7 +1722,7 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="23"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1734,7 +1734,7 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="23"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1746,7 +1746,7 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="23"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
@@ -1768,7 +1768,7 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1792,7 +1792,7 @@
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="23"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
@@ -1814,7 +1814,7 @@
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="23"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1888,11 +1888,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1900,6 +1895,11 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1925,7 +1925,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>89</v>
       </c>
       <c r="B1" s="33"/>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="34" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -1960,7 +1960,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>4</v>
@@ -1977,12 +1977,12 @@
         <v>5</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>65</v>
@@ -1996,7 +1996,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>65</v>
@@ -2010,7 +2010,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>65</v>
@@ -2024,7 +2024,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>65</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>65</v>
@@ -2052,7 +2052,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>65</v>
@@ -2066,7 +2066,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>65</v>
@@ -2080,7 +2080,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>65</v>
@@ -2094,7 +2094,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>65</v>
@@ -2108,7 +2108,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>65</v>
@@ -2122,7 +2122,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>65</v>
@@ -2136,7 +2136,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>65</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>65</v>
@@ -2164,7 +2164,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>65</v>
@@ -2178,7 +2178,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>65</v>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>65</v>
@@ -2206,7 +2206,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>65</v>
@@ -2220,13 +2220,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>64</v>
@@ -2234,7 +2234,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>64</v>
@@ -2248,7 +2248,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>64</v>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
-Actualización y finalización de la Especificación del CU Revisar Programa.
-Elaboración del diagrama de secuencia del CU Revisar Programa.

-Actualización del documento: Seguimiento Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -357,7 +357,7 @@
     <t>Ver Vigencia de Programas</t>
   </si>
   <si>
-    <t>En total se encuentran finalizados 18 de 21 Documentos de Especificación.</t>
+    <t>En total se encuentran finalizados 19 de 21 Documentos de Especificación.</t>
   </si>
 </sst>
 </file>
@@ -581,9 +581,30 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -591,27 +612,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -950,15 +950,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -968,29 +968,29 @@
       <c r="N1" s="12"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="27" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="24" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="30"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
@@ -1000,11 +1000,11 @@
       <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="27"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1028,7 +1028,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1072,7 +1072,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1094,7 +1094,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1116,7 +1116,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1138,7 +1138,7 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1160,7 +1160,7 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1182,7 +1182,7 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1218,7 +1218,7 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="22"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="22"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1262,7 +1262,7 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="22"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="22"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1296,7 +1296,7 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="22"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="22"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1320,7 +1320,7 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="22"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1332,7 +1332,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="22"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="22"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="22"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="22"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1410,7 +1410,7 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="22"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="22"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1434,7 +1434,7 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="22"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="22"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="22"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1480,7 +1480,7 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="22"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1502,7 +1502,7 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="22"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
@@ -1524,7 +1524,7 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="22"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1546,7 +1546,7 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="23" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1560,7 +1560,7 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="22"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1572,7 +1572,7 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="22"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1584,7 +1584,7 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="30" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1608,7 +1608,7 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="24"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1630,7 +1630,7 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="24"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
@@ -1652,7 +1652,7 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="25"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1698,7 +1698,7 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1722,7 +1722,7 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="22"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1734,7 +1734,7 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="22"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1746,7 +1746,7 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="22"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
@@ -1768,7 +1768,7 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1792,7 +1792,7 @@
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="22"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
@@ -1814,7 +1814,7 @@
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="22"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1888,6 +1888,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1895,11 +1900,6 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1925,7 +1925,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>89</v>
       </c>
       <c r="B1" s="33"/>
@@ -2237,10 +2237,10 @@
         <v>110</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
-Actualización y completado del Documento de Especificación del CU Ver Vigencia de Programas.
-Elaboración del Diagrama de Secuencia del CU Ver Vigencia de Programas.

-Actualización del Diagrama de CU Individual del CU Ver Vigencia de Programas.

-Actualización del Documento de Segumiento de Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -357,7 +357,7 @@
     <t>Ver Vigencia de Programas</t>
   </si>
   <si>
-    <t>En total se encuentran finalizados 19 de 21 Documentos de Especificación.</t>
+    <t>En total se encuentran finalizados 20 de 21 Documentos de Especificación.</t>
   </si>
 </sst>
 </file>
@@ -581,12 +581,21 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -603,15 +612,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -950,15 +950,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -968,29 +968,29 @@
       <c r="N1" s="12"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="24" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="27" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="27"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
@@ -1000,11 +1000,11 @@
       <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1028,7 +1028,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="23"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="23"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1072,7 +1072,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="23"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1094,7 +1094,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="23"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1116,7 +1116,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="23"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1138,7 +1138,7 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="23"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1160,7 +1160,7 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="23"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1182,7 +1182,7 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="23"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1218,7 +1218,7 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="23"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="23"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1262,7 +1262,7 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="23"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="23"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1296,7 +1296,7 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="23"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="23"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1320,7 +1320,7 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="23"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1332,7 +1332,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="23"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="23"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="23"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="23"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1410,7 +1410,7 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="23"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="23"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1434,7 +1434,7 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="23"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="23"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="23"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1480,7 +1480,7 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="23"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1502,7 +1502,7 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="23"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
@@ -1524,7 +1524,7 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="23"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1546,7 +1546,7 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1560,7 +1560,7 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="23"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1572,7 +1572,7 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="23"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1584,7 +1584,7 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="23" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1608,7 +1608,7 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="31"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1630,7 +1630,7 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="31"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
@@ -1652,7 +1652,7 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="32"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1698,7 +1698,7 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1722,7 +1722,7 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="23"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1734,7 +1734,7 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="23"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1746,7 +1746,7 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="23"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
@@ -1768,7 +1768,7 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1792,7 +1792,7 @@
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="23"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
@@ -1814,7 +1814,7 @@
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="23"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1888,11 +1888,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1900,6 +1895,11 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1925,7 +1925,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>89</v>
       </c>
       <c r="B1" s="33"/>
@@ -2265,13 +2265,13 @@
         <v>112</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Actualización y completado de secciones del Manual de Usuario.
-Actualización y agregación de capturas de pantalla de los CU.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -581,9 +581,30 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -591,27 +612,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -950,15 +950,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -968,29 +968,29 @@
       <c r="N1" s="12"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="27" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="24" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="30"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
@@ -1000,11 +1000,11 @@
       <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="27"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1028,7 +1028,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1050,7 +1050,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1072,7 +1072,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1094,7 +1094,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1116,7 +1116,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1138,7 +1138,7 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1160,7 +1160,7 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1182,7 +1182,7 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1194,7 +1194,7 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1218,7 +1218,7 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="22"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1240,7 +1240,7 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="22"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1262,7 +1262,7 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="22"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="22"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1296,7 +1296,7 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="22"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1308,7 +1308,7 @@
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="22"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1320,7 +1320,7 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="22"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1332,7 +1332,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="22"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="22"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1376,7 +1376,7 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="22"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="22"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1410,7 +1410,7 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="22"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="22"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1434,7 +1434,7 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="22"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1446,7 +1446,7 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="22"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="22"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1480,7 +1480,7 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="22"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1502,7 +1502,7 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="22"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
@@ -1524,7 +1524,7 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="22"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1546,7 +1546,7 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="23" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1560,7 +1560,7 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="22"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1572,7 +1572,7 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="22"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1584,7 +1584,7 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="30" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1597,10 +1597,10 @@
         <v>64</v>
       </c>
       <c r="E37" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>85</v>
@@ -1608,7 +1608,7 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="24"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1630,7 +1630,7 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="24"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
@@ -1652,7 +1652,7 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="25"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1698,7 +1698,7 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1722,7 +1722,7 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="22"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1734,7 +1734,7 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="22"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1746,7 +1746,7 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="22"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
@@ -1768,7 +1768,7 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1792,7 +1792,7 @@
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="22"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
@@ -1814,7 +1814,7 @@
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="22"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1888,6 +1888,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1895,11 +1900,6 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1925,7 +1925,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>89</v>
       </c>
       <c r="B1" s="33"/>

</xml_diff>

<commit_message>
-Elaboración de la Especificación del CU Generar Informe Gerencial.
-Corrección de mensajes en los CU Subir Plan, Subir Programa, Carga Masiva de Programas y Gestionar Carrera.

-Actualización del Documento: Seguimiento Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="115">
   <si>
     <t>DOCUMENTACIÓN - METODOLOGÍA DE DESARROLLO PSI</t>
   </si>
@@ -357,7 +357,10 @@
     <t>Ver Vigencia de Programas</t>
   </si>
   <si>
-    <t>En total se encuentran finalizados 20 de 21 Documentos de Especificación.</t>
+    <t>SI (Se debe actualizar)</t>
+  </si>
+  <si>
+    <t>En total se encuentran finalizados 17 de 21 Documentos de Especificación.</t>
   </si>
 </sst>
 </file>
@@ -1944,7 +1947,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="34" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -1985,10 +1988,10 @@
         <v>92</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>64</v>
@@ -2013,10 +2016,10 @@
         <v>94</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>64</v>
@@ -2237,10 +2240,10 @@
         <v>110</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>64</v>
+        <v>113</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>64</v>
@@ -2254,10 +2257,10 @@
         <v>64</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4">

</xml_diff>

<commit_message>
-Elaboración del Diagrama de Secuencia del CU Generar Informe Gerencial. -Finalización de la Especificación del CU Generar Informe Gerencial. -Actualización del Documento Seguimiento de Documentación. -Corrección de Permisos del botón Ir a Panel principal SA.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -360,7 +360,7 @@
     <t>SI (Se debe actualizar)</t>
   </si>
   <si>
-    <t>En total se encuentran finalizados 17 de 21 Documentos de Especificación.</t>
+    <t>En total se encuentran finalizados 18 de 21 Documentos de Especificación.</t>
   </si>
 </sst>
 </file>
@@ -584,12 +584,21 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -606,15 +615,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -953,15 +953,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -971,29 +971,29 @@
       <c r="N1" s="12"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="24" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="27" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="27"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
@@ -1003,11 +1003,11 @@
       <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1031,7 +1031,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="23"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1053,7 +1053,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="23"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1075,7 +1075,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="23"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1097,7 +1097,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="23"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1119,7 +1119,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="23"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="23"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1163,7 +1163,7 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="23"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1185,7 +1185,7 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="23"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1197,7 +1197,7 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1221,7 +1221,7 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="23"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1243,7 +1243,7 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="23"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="23"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1277,7 +1277,7 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="23"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1299,7 +1299,7 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="23"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1311,7 +1311,7 @@
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="23"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1323,7 +1323,7 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="23"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="23"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1357,7 +1357,7 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="23"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1379,7 +1379,7 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="23"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1401,7 +1401,7 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="23"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1413,7 +1413,7 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="23"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1425,7 +1425,7 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="23"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="23"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1449,7 +1449,7 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="23"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1461,7 +1461,7 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="23"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1483,7 +1483,7 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="23"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1505,7 +1505,7 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="23"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
@@ -1527,7 +1527,7 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="23"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1549,7 +1549,7 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1563,7 +1563,7 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="23"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1575,7 +1575,7 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="23"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1587,7 +1587,7 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="23" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1611,7 +1611,7 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="31"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1633,7 +1633,7 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="31"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
@@ -1655,7 +1655,7 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="32"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1701,7 +1701,7 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1725,7 +1725,7 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="23"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1737,7 +1737,7 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="23"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1749,7 +1749,7 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="23"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
@@ -1771,7 +1771,7 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1795,7 +1795,7 @@
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="23"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
@@ -1817,7 +1817,7 @@
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="23"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1891,11 +1891,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1903,6 +1898,11 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1928,7 +1928,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>89</v>
       </c>
       <c r="B1" s="33"/>
@@ -2254,10 +2254,10 @@
         <v>111</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
-Elaboración e inicio del Glosario del sistema.
-Actualización del documento: Seguimiento Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -584,9 +584,30 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -594,27 +615,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -953,15 +953,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -971,29 +971,29 @@
       <c r="N1" s="12"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="27" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="24" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="30"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
@@ -1003,11 +1003,11 @@
       <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="27"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1031,7 +1031,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1053,7 +1053,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1075,7 +1075,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1097,7 +1097,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1119,7 +1119,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1141,7 +1141,7 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1163,7 +1163,7 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1185,7 +1185,7 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1197,7 +1197,7 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1221,7 +1221,7 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="22"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1243,7 +1243,7 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="22"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="22"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1277,7 +1277,7 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="22"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1299,7 +1299,7 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="22"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1311,7 +1311,7 @@
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="22"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1323,7 +1323,7 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="22"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="22"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1357,7 +1357,7 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="22"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1379,7 +1379,7 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="22"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1401,7 +1401,7 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="22"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1413,7 +1413,7 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="22"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1425,7 +1425,7 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="22"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1437,7 +1437,7 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="22"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1449,7 +1449,7 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="22"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1461,7 +1461,7 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="22"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1483,7 +1483,7 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="22"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1505,7 +1505,7 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="22"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
@@ -1527,7 +1527,7 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="22"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1549,7 +1549,7 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="23" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1563,7 +1563,7 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="22"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1575,7 +1575,7 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="22"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1587,7 +1587,7 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="30" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1611,7 +1611,7 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="24"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1622,10 +1622,10 @@
         <v>64</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G38" s="9" t="s">
         <v>85</v>
@@ -1633,7 +1633,7 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="24"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
@@ -1655,7 +1655,7 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="25"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1701,7 +1701,7 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1725,7 +1725,7 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="22"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1737,7 +1737,7 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="22"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1749,7 +1749,7 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="22"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
@@ -1771,7 +1771,7 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1795,7 +1795,7 @@
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="22"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
@@ -1817,7 +1817,7 @@
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="22"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1891,6 +1891,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1898,11 +1903,6 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1928,7 +1928,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>89</v>
       </c>
       <c r="B1" s="33"/>

</xml_diff>

<commit_message>
-Actualización de las especificaciones de los CU:
Gestionar Asignatura, Gestionar Programa y Revisar Programa.

-Actualización de diagramas de CU y de Secuencia asociados.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -360,7 +360,7 @@
     <t>SI (Se debe actualizar)</t>
   </si>
   <si>
-    <t>En total se encuentran finalizados 18 de 21 Documentos de Especificación.</t>
+    <t>En total se encuentran finalizados 20 de 21 Documentos de Especificación.</t>
   </si>
 </sst>
 </file>
@@ -1917,7 +1917,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1988,10 +1988,10 @@
         <v>92</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>64</v>
@@ -2240,10 +2240,10 @@
         <v>110</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
-Actualización de diagramas de secuencia.
-Actualización y finalización de los 21 documentos de especificación de CU.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="114">
   <si>
     <t>DOCUMENTACIÓN - METODOLOGÍA DE DESARROLLO PSI</t>
   </si>
@@ -357,10 +357,7 @@
     <t>Ver Vigencia de Programas</t>
   </si>
   <si>
-    <t>SI (Se debe actualizar)</t>
-  </si>
-  <si>
-    <t>En total se encuentran finalizados 20 de 21 Documentos de Especificación.</t>
+    <t>En total se encuentran finalizados 21 de 21 Documentos de Especificación.</t>
   </si>
 </sst>
 </file>
@@ -584,12 +581,21 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -606,15 +612,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -953,15 +950,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -971,29 +968,29 @@
       <c r="N1" s="12"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="24" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="27" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="27"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
@@ -1003,11 +1000,11 @@
       <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1017,10 +1014,10 @@
         <v>70</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>64</v>
@@ -1031,7 +1028,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="23"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1053,7 +1050,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="23"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1075,7 +1072,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="23"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1097,7 +1094,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="23"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1119,7 +1116,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="23"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1141,7 +1138,7 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="23"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1163,7 +1160,7 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="23"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1185,7 +1182,7 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="23"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1197,7 +1194,7 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1221,7 +1218,7 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="23"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1243,7 +1240,7 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="23"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1265,7 +1262,7 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="23"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1277,7 +1274,7 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="23"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1299,7 +1296,7 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="23"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1311,7 +1308,7 @@
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="23"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1323,7 +1320,7 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="23"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1335,7 +1332,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="23"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1357,7 +1354,7 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="23"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1379,7 +1376,7 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="23"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1401,7 +1398,7 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="23"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1413,7 +1410,7 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="23"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1425,7 +1422,7 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="23"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1437,7 +1434,7 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="23"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1449,7 +1446,7 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="23"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1461,7 +1458,7 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="23"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1483,7 +1480,7 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="23"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1505,7 +1502,7 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="23"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
@@ -1527,7 +1524,7 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="23"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1549,7 +1546,7 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1563,7 +1560,7 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="23"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1575,7 +1572,7 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="23"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1587,7 +1584,7 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="23" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1611,7 +1608,7 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="31"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1633,7 +1630,7 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="31"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
@@ -1655,7 +1652,7 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="32"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1701,7 +1698,7 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1725,7 +1722,7 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="23"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1737,7 +1734,7 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="23"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1749,7 +1746,7 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="23"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
@@ -1771,7 +1768,7 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1795,7 +1792,7 @@
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="23"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
@@ -1817,7 +1814,7 @@
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="23"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1891,11 +1888,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1903,6 +1895,11 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1917,7 +1914,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1928,7 +1925,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>89</v>
       </c>
       <c r="B1" s="33"/>
@@ -1947,7 +1944,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -2016,10 +2013,10 @@
         <v>94</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
-Actualización de la redacción del listado de permisos del sistema.
-Actualización y finalización del Documento Arquitectura del Sistema.

-Actualización y finalización del Documento Modelo de Datos.

-Aporte de valoraciones personales en la Memoria del Proyecto.

-Actualización del Seguimiento de Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="113">
   <si>
     <t>DOCUMENTACIÓN - METODOLOGÍA DE DESARROLLO PSI</t>
   </si>
@@ -277,9 +277,6 @@
   </si>
   <si>
     <t>SI (actualizar antes de entregar)</t>
-  </si>
-  <si>
-    <t>SI (actualizar)</t>
   </si>
   <si>
     <t>Francisco Estrada y Fabricio González</t>
@@ -1080,7 +1077,7 @@
         <v>70</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>64</v>
@@ -1102,7 +1099,7 @@
         <v>70</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>64</v>
@@ -1463,7 +1460,7 @@
         <v>33</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>65</v>
@@ -1926,7 +1923,7 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -1944,7 +1941,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -1960,7 +1957,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>4</v>
@@ -1977,12 +1974,12 @@
         <v>5</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>65</v>
@@ -1996,7 +1993,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>65</v>
@@ -2010,7 +2007,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>65</v>
@@ -2024,7 +2021,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>65</v>
@@ -2038,7 +2035,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>65</v>
@@ -2052,7 +2049,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>65</v>
@@ -2066,7 +2063,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>65</v>
@@ -2080,7 +2077,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>65</v>
@@ -2094,7 +2091,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>65</v>
@@ -2108,7 +2105,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>65</v>
@@ -2122,7 +2119,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>65</v>
@@ -2136,7 +2133,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>65</v>
@@ -2150,7 +2147,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>65</v>
@@ -2164,7 +2161,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>65</v>
@@ -2178,7 +2175,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>65</v>
@@ -2192,7 +2189,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>65</v>
@@ -2206,7 +2203,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>65</v>
@@ -2220,7 +2217,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>65</v>
@@ -2234,7 +2231,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>65</v>
@@ -2248,7 +2245,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>65</v>
@@ -2262,7 +2259,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
-Elaboración de los Casos de Prueba del CU Generar Informe Gerencial.
-Actualización de los Casos de Prueba de los CU Enviar Notificación y Ver Vigencia de Programas.

-Actualización del Seguimiento de Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -578,9 +578,30 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -588,27 +609,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -947,15 +947,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -965,29 +965,29 @@
       <c r="N1" s="12"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="27" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="24" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="30"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
@@ -997,11 +997,11 @@
       <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="27"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1025,7 +1025,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1091,7 +1091,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1113,7 +1113,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1135,7 +1135,7 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1157,7 +1157,7 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1191,7 +1191,7 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1215,7 +1215,7 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="22"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1237,7 +1237,7 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="22"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="22"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1271,7 +1271,7 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="22"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="22"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1305,7 +1305,7 @@
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="22"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1317,7 +1317,7 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="22"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1329,7 +1329,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="22"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1351,7 +1351,7 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="22"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="22"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1395,7 +1395,7 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="22"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1407,7 +1407,7 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="22"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1419,7 +1419,7 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="22"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1431,7 +1431,7 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="22"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1443,7 +1443,7 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="22"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="22"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1477,7 +1477,7 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="22"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1499,7 +1499,7 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="22"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
@@ -1521,7 +1521,7 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="22"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1543,7 +1543,7 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="23" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1557,7 +1557,7 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="22"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1569,7 +1569,7 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="22"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1581,7 +1581,7 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="30" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1605,7 +1605,7 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="24"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1613,10 +1613,10 @@
         <v>76</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>64</v>
@@ -1627,7 +1627,7 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="24"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
@@ -1649,7 +1649,7 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="25"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1695,7 +1695,7 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1719,7 +1719,7 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="22"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1731,7 +1731,7 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="22"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1743,7 +1743,7 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="22"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
@@ -1765,7 +1765,7 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1789,7 +1789,7 @@
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="22"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
@@ -1811,7 +1811,7 @@
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="22"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1885,6 +1885,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1892,11 +1897,6 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1922,7 +1922,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>88</v>
       </c>
       <c r="B1" s="33"/>

</xml_diff>

<commit_message>
-Completado de secciones de la Memoria del Proyecto.
-Actualización del Seguimiento de Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -578,12 +578,21 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,15 +609,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -947,15 +947,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -965,29 +965,29 @@
       <c r="N1" s="12"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="24" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="27" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="27"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
@@ -997,11 +997,11 @@
       <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1025,7 +1025,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="23"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="23"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="23"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1091,7 +1091,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="23"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1113,7 +1113,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="23"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1135,7 +1135,7 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="23"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1157,7 +1157,7 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="23"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="23"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1191,7 +1191,7 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1215,7 +1215,7 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="23"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1237,7 +1237,7 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="23"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="23"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1271,7 +1271,7 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="23"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="23"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1305,7 +1305,7 @@
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="23"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1317,7 +1317,7 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="23"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1329,7 +1329,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="23"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1351,7 +1351,7 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="23"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="23"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1395,7 +1395,7 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="23"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1407,7 +1407,7 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="23"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1419,7 +1419,7 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="23"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1431,7 +1431,7 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="23"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1443,7 +1443,7 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="23"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="23"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1477,7 +1477,7 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="23"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1499,7 +1499,7 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="23"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
@@ -1521,7 +1521,7 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="23"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1543,7 +1543,7 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1557,7 +1557,7 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="23"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1569,7 +1569,7 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="23"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1581,7 +1581,7 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="23" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1605,7 +1605,7 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="31"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1627,7 +1627,7 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="31"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
@@ -1638,10 +1638,10 @@
         <v>64</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G39" s="9" t="s">
         <v>85</v>
@@ -1649,7 +1649,7 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="32"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1695,7 +1695,7 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1719,7 +1719,7 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="23"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1731,7 +1731,7 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="23"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1743,7 +1743,7 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="23"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
@@ -1765,7 +1765,7 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1789,7 +1789,7 @@
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="23"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
@@ -1811,7 +1811,7 @@
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="23"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1885,11 +1885,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1897,6 +1892,11 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1922,7 +1922,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>88</v>
       </c>
       <c r="B1" s="33"/>

</xml_diff>

<commit_message>
-Actualización y completado de secciones en la Memoria del Proyecto.
-Actualización del seguimiento de documentación y pruebas del sistema.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -578,9 +578,30 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -588,27 +609,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -947,15 +947,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -965,29 +965,29 @@
       <c r="N1" s="12"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="27" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="24" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="30"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
@@ -997,11 +997,11 @@
       <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="27"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1025,7 +1025,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1091,7 +1091,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1113,7 +1113,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1135,7 +1135,7 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1157,7 +1157,7 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1191,7 +1191,7 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1215,7 +1215,7 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="22"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1237,7 +1237,7 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="22"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="22"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1271,7 +1271,7 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="22"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="22"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1305,7 +1305,7 @@
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="22"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1317,7 +1317,7 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="22"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1329,7 +1329,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="22"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1351,7 +1351,7 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="22"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="22"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1395,7 +1395,7 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="22"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1407,7 +1407,7 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="22"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1419,7 +1419,7 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="22"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1431,7 +1431,7 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="22"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1443,7 +1443,7 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="22"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="22"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1477,7 +1477,7 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="22"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1499,7 +1499,7 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="22"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
@@ -1521,7 +1521,7 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="22"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1543,7 +1543,7 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="23" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1557,7 +1557,7 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="22"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1569,7 +1569,7 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="22"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1581,7 +1581,7 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="30" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1605,7 +1605,7 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="24"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1627,7 +1627,7 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="24"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
@@ -1635,10 +1635,10 @@
         <v>76</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>64</v>
@@ -1649,7 +1649,7 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="25"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1695,7 +1695,7 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1719,7 +1719,7 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="22"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1731,7 +1731,7 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="22"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1743,7 +1743,7 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="22"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
@@ -1765,7 +1765,7 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1789,7 +1789,7 @@
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="22"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
@@ -1811,7 +1811,7 @@
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="22"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1885,6 +1885,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1892,11 +1897,6 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1922,7 +1922,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>88</v>
       </c>
       <c r="B1" s="33"/>

</xml_diff>

<commit_message>
-Realización de pruebas iniciales al CU Generar Informe Gerencial.
-Actualización de los documentos de seguimiento de Pruebas y Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -578,12 +578,21 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -600,15 +609,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -947,15 +947,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -965,29 +965,29 @@
       <c r="N1" s="12"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="24" t="s">
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="27" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="27"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
@@ -997,11 +997,11 @@
       <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="24"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1025,7 +1025,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="23"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="23"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="23"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1091,7 +1091,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="23"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1113,7 +1113,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="23"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1135,7 +1135,7 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="23"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1157,7 +1157,7 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="23"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="23"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1191,7 +1191,7 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1215,7 +1215,7 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="23"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1237,7 +1237,7 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="23"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1259,7 +1259,7 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="23"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1271,7 +1271,7 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="23"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1293,7 +1293,7 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="23"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1305,7 +1305,7 @@
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="23"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1317,7 +1317,7 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="23"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1329,7 +1329,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="23"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1351,7 +1351,7 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="23"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1373,7 +1373,7 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="23"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1395,7 +1395,7 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="23"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1407,7 +1407,7 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="23"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1419,7 +1419,7 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="23"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1431,7 +1431,7 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="23"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1443,7 +1443,7 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="23"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="23"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1477,7 +1477,7 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="23"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1499,7 +1499,7 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="23"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
@@ -1521,7 +1521,7 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="23"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1543,7 +1543,7 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1557,7 +1557,7 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="23"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1569,7 +1569,7 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="23"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1581,7 +1581,7 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="23" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1605,7 +1605,7 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="31"/>
+      <c r="A38" s="24"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1627,7 +1627,7 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="31"/>
+      <c r="A39" s="24"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
@@ -1649,7 +1649,7 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="32"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1695,7 +1695,7 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1705,10 +1705,10 @@
         <v>70</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>64</v>
@@ -1719,7 +1719,7 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="23"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1731,7 +1731,7 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="23"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1743,7 +1743,7 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="23"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
@@ -1765,7 +1765,7 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1789,7 +1789,7 @@
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="23"/>
+      <c r="A47" s="22"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
@@ -1811,7 +1811,7 @@
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="23"/>
+      <c r="A48" s="22"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1885,11 +1885,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1897,6 +1892,11 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1922,7 +1922,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>88</v>
       </c>
       <c r="B1" s="33"/>

</xml_diff>

<commit_message>
- Completado de la Sección "Introducción al Sistema" del Manual de Usuario.
- Actualización del Seguimiento de Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="112">
   <si>
     <t>DOCUMENTACIÓN - METODOLOGÍA DE DESARROLLO PSI</t>
   </si>
@@ -274,9 +274,6 @@
   </si>
   <si>
     <t>SI (/Manuales)</t>
-  </si>
-  <si>
-    <t>SI (actualizar antes de entregar)</t>
   </si>
   <si>
     <t>Francisco Estrada y Fabricio González</t>
@@ -578,9 +575,30 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -588,27 +606,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -947,15 +944,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
       <c r="J1" s="12"/>
@@ -965,29 +962,29 @@
       <c r="N1" s="12"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="27" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="24" t="s">
         <v>57</v>
       </c>
       <c r="H3" s="11"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="30"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
@@ -997,11 +994,11 @@
       <c r="F4" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="27"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1025,7 +1022,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1047,7 +1044,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1069,7 +1066,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1091,7 +1088,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1113,7 +1110,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1135,7 +1132,7 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1157,7 +1154,7 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1179,7 +1176,7 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1191,7 +1188,7 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="23" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1215,7 +1212,7 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="22"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1237,7 +1234,7 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="22"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1259,7 +1256,7 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="22"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1271,7 +1268,7 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="22"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1293,7 +1290,7 @@
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="22"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1305,7 +1302,7 @@
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="22"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1317,7 +1314,7 @@
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="22"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1329,7 +1326,7 @@
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="22"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1351,7 +1348,7 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="22"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1373,7 +1370,7 @@
       <c r="H23" s="10"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="22"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1395,7 +1392,7 @@
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="22"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1407,7 +1404,7 @@
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="22"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1419,7 +1416,7 @@
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="22"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1431,7 +1428,7 @@
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="22"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1443,7 +1440,7 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="22"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1455,12 +1452,12 @@
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="22"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>65</v>
@@ -1477,7 +1474,7 @@
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="22"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1499,7 +1496,7 @@
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="22"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
@@ -1521,7 +1518,7 @@
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="22"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1543,7 +1540,7 @@
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="23" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1557,7 +1554,7 @@
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="22"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1569,7 +1566,7 @@
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="22"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1581,7 +1578,7 @@
       <c r="H36" s="10"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="30" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
@@ -1605,7 +1602,7 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="24"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1627,7 +1624,7 @@
       <c r="H38" s="10"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="24"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
@@ -1649,7 +1646,7 @@
       <c r="H39" s="10"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="25"/>
+      <c r="A40" s="32"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1681,7 +1678,7 @@
         <v>77</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>64</v>
@@ -1695,7 +1692,7 @@
       <c r="H41" s="10"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="22" t="s">
+      <c r="A42" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1719,7 +1716,7 @@
       <c r="H42" s="10"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="22"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1731,7 +1728,7 @@
       <c r="H43" s="10"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="22"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1743,7 +1740,7 @@
       <c r="H44" s="10"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="22"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
@@ -1765,7 +1762,7 @@
       <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="23" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1789,7 +1786,7 @@
       <c r="H46" s="10"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="22"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
@@ -1811,7 +1808,7 @@
       <c r="H47" s="10"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="22"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1885,6 +1882,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="G3:G4"/>
@@ -1892,11 +1894,6 @@
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1922,8 +1919,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="26" t="s">
-        <v>88</v>
+      <c r="A1" s="22" t="s">
+        <v>87</v>
       </c>
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
@@ -1941,7 +1938,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -1957,7 +1954,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>4</v>
@@ -1974,12 +1971,12 @@
         <v>5</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>65</v>
@@ -1993,7 +1990,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>65</v>
@@ -2007,7 +2004,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>65</v>
@@ -2021,7 +2018,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>65</v>
@@ -2035,7 +2032,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>65</v>
@@ -2049,7 +2046,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>65</v>
@@ -2063,7 +2060,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>65</v>
@@ -2077,7 +2074,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>65</v>
@@ -2091,7 +2088,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>65</v>
@@ -2105,7 +2102,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>65</v>
@@ -2119,7 +2116,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>65</v>
@@ -2133,7 +2130,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>65</v>
@@ -2147,7 +2144,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>65</v>
@@ -2161,7 +2158,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>65</v>
@@ -2175,7 +2172,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>65</v>
@@ -2189,7 +2186,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>65</v>
@@ -2203,7 +2200,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>65</v>
@@ -2217,7 +2214,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>65</v>
@@ -2231,7 +2228,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>65</v>
@@ -2245,7 +2242,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>65</v>
@@ -2259,7 +2256,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
-Actualización de capturas de pantalla de los CU.
-Actualización del Manual de Usuario.

-Actualización del Seguimiento de Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="102">
   <si>
     <t>DOCUMENTACIÓN - METODOLOGÍA DE DESARROLLO PSI</t>
   </si>
@@ -189,9 +189,6 @@
     <t xml:space="preserve">NOTA: Me guié de las plantillas.dotx que habiamos descargado el año pasado. Ya que la página PSI no funciona adecuadamente. </t>
   </si>
   <si>
-    <t>¿Se encuentra en GIT?</t>
-  </si>
-  <si>
     <t>Los documentos que se piden en la planificacion del 2018 y que no se encuentran en las plantillas son el Modelo de componentes y Clases de Diseño.</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t xml:space="preserve">Fabricio Gonzalez </t>
   </si>
   <si>
-    <t>SI (/inicio)</t>
-  </si>
-  <si>
     <t>Fabricio Gonzalez y Nicolás Sartini</t>
   </si>
   <si>
@@ -231,21 +225,9 @@
     <t>Nicolás Sartini</t>
   </si>
   <si>
-    <t>SI (/inicio y /Elaboracion)</t>
-  </si>
-  <si>
     <t>Francisco Estrada</t>
   </si>
   <si>
-    <t>SI (/Elaboracion)</t>
-  </si>
-  <si>
-    <t>SI (/Construcción)</t>
-  </si>
-  <si>
-    <t>SI (/Elaboracion y /Construccion)</t>
-  </si>
-  <si>
     <t>Fabricio Gonzalez, Nicolás Sartini y Francisco Estrada</t>
   </si>
   <si>
@@ -258,22 +240,10 @@
     <t>Prototipos de Interfaz</t>
   </si>
   <si>
-    <t>SI (/Elaboración y /Construcción)</t>
-  </si>
-  <si>
-    <t>SI (/inicio , /Elaboración y /Construcción)</t>
-  </si>
-  <si>
-    <t>SI (/inicio y /Construcción)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Los que estan resaltados en amarillo son los documentos que se piden en la planificacion del 2018 y por lo tanto, son obligatorios. </t>
   </si>
   <si>
     <t>Memoria del Proyecto</t>
-  </si>
-  <si>
-    <t>SI (/Manuales)</t>
   </si>
   <si>
     <t>Francisco Estrada y Fabricio González</t>
@@ -518,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -545,7 +515,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -572,8 +541,17 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -581,10 +559,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -936,611 +914,571 @@
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
     <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="44.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="H3" s="11"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="27"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="16" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="11"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H5" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="23"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="23"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H6" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="23"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="23"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H7" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="23"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="23"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H9" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="23"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="23"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="23"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="23"/>
+      <c r="H11" s="14"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="25"/>
+      <c r="B12" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="23"/>
-      <c r="B12" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H12" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="23"/>
+      <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="23"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="H14" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="23"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="23"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="23"/>
+      <c r="H16" s="14"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="23"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="10"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="23"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H18" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="23"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="23"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="10"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="23"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="23"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="H22" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" s="23"/>
+      <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="23"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="H23" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="23"/>
+      <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="23"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>64</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="H24" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="23"/>
+      <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="23"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="10"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="23"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="10"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="23"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="23"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="10"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="14"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="23"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="10"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="23"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H30" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" s="23"/>
+      <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="23"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H31" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="23"/>
+      <c r="H31" s="14"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="23"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="H32" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" s="23"/>
+      <c r="H32" s="14"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="23"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H33" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="23"/>
+      <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="25" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1549,123 +1487,115 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="10"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="14"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="23"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="10"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="14"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="23"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="10"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="14"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="14" t="s">
-        <v>84</v>
+      <c r="B37" s="13" t="s">
+        <v>75</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H37" s="10"/>
+        <v>70</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" s="23"/>
+      <c r="H37" s="14"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="31"/>
+      <c r="A38" s="33"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="H38" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38" s="23"/>
+      <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="31"/>
+      <c r="A39" s="33"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="H39" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G39" s="23"/>
+      <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="32"/>
+      <c r="A40" s="34"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="H40" s="10"/>
+        <v>64</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G40" s="23"/>
+      <c r="H40" s="14"/>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="2" t="s">
@@ -1675,164 +1605,154 @@
         <v>46</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="H41" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G41" s="23"/>
+      <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="25" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H42" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G42" s="23"/>
+      <c r="H42" s="14"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="23"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="10"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="23"/>
+      <c r="H43" s="14"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="23"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="10"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="14"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="23"/>
+      <c r="A45" s="25"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="H45" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G45" s="23"/>
+      <c r="H45" s="14"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="25" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G46" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="H46" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G46" s="23"/>
+      <c r="H46" s="14"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="23"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G47" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="H47" s="10"/>
+        <v>63</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47" s="23"/>
+      <c r="H47" s="14"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="23"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="10"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="14"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>58</v>
-      </c>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
+        <v>57</v>
+      </c>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1842,27 +1762,27 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -1881,7 +1801,7 @@
       <c r="A69" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="11">
     <mergeCell ref="A14:A33"/>
     <mergeCell ref="A34:A36"/>
     <mergeCell ref="A42:A45"/>
@@ -1889,7 +1809,6 @@
     <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
-    <mergeCell ref="G3:G4"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
@@ -1919,353 +1838,353 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="22" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="33"/>
+      <c r="A1" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
+      <c r="A4" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7" s="36" t="s">
+      <c r="A7" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="35"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="37"/>
+      <c r="B8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>89</v>
+      <c r="D8" s="18" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="3" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="3" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="3" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="3" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="3" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Finalización del Manual de Usuario.
-Actualización del Seguimiento de Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -553,12 +553,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -575,15 +584,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -922,15 +922,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
@@ -940,27 +940,27 @@
       <c r="N1" s="11"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="10"/>
       <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="29"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="29"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="32"/>
       <c r="D4" s="15" t="s">
         <v>6</v>
       </c>
@@ -974,7 +974,7 @@
       <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -996,7 +996,7 @@
       <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="25"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1016,7 +1016,7 @@
       <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="25"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1036,7 +1036,7 @@
       <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="25"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1056,7 +1056,7 @@
       <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="25"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1076,7 +1076,7 @@
       <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="25"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1096,7 +1096,7 @@
       <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="25"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1116,7 +1116,7 @@
       <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="25"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="4" t="s">
         <v>73</v>
       </c>
@@ -1136,7 +1136,7 @@
       <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="25"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1148,7 +1148,7 @@
       <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1170,7 +1170,7 @@
       <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="25"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1190,7 +1190,7 @@
       <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="25"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
@@ -1210,7 +1210,7 @@
       <c r="H16" s="14"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="25"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1222,7 +1222,7 @@
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="25"/>
+      <c r="A18" s="24"/>
       <c r="B18" s="5" t="s">
         <v>72</v>
       </c>
@@ -1242,7 +1242,7 @@
       <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="25"/>
+      <c r="A19" s="24"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1254,7 +1254,7 @@
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="25"/>
+      <c r="A20" s="24"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1266,7 +1266,7 @@
       <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="25"/>
+      <c r="A21" s="24"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1278,7 +1278,7 @@
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="25"/>
+      <c r="A22" s="24"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1298,7 +1298,7 @@
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="25"/>
+      <c r="A23" s="24"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
@@ -1318,7 +1318,7 @@
       <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="25"/>
+      <c r="A24" s="24"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
@@ -1338,7 +1338,7 @@
       <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="25"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1350,7 +1350,7 @@
       <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="25"/>
+      <c r="A26" s="24"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1362,7 +1362,7 @@
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="25"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1374,7 +1374,7 @@
       <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="25"/>
+      <c r="A28" s="24"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1386,7 +1386,7 @@
       <c r="H28" s="14"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="25"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="25"/>
+      <c r="A30" s="24"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1418,7 +1418,7 @@
       <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="25"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1438,7 +1438,7 @@
       <c r="H31" s="14"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="25"/>
+      <c r="A32" s="24"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
@@ -1458,7 +1458,7 @@
       <c r="H32" s="14"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="25"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
@@ -1478,7 +1478,7 @@
       <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="24" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1492,7 +1492,7 @@
       <c r="H34" s="14"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="25"/>
+      <c r="A35" s="24"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1504,7 +1504,7 @@
       <c r="H35" s="14"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="25"/>
+      <c r="A36" s="24"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1516,7 +1516,7 @@
       <c r="H36" s="14"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="25" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="13" t="s">
@@ -1538,7 +1538,7 @@
       <c r="H37" s="14"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="33"/>
+      <c r="A38" s="26"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
@@ -1558,7 +1558,7 @@
       <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="33"/>
+      <c r="A39" s="26"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
@@ -1578,7 +1578,7 @@
       <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="34"/>
+      <c r="A40" s="27"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
@@ -1586,10 +1586,10 @@
         <v>70</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>63</v>
@@ -1620,7 +1620,7 @@
       <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="24" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1642,7 +1642,7 @@
       <c r="H42" s="14"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="25"/>
+      <c r="A43" s="24"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1654,7 +1654,7 @@
       <c r="H43" s="14"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="25"/>
+      <c r="A44" s="24"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1666,7 +1666,7 @@
       <c r="H44" s="14"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="25"/>
+      <c r="A45" s="24"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
@@ -1686,7 +1686,7 @@
       <c r="H45" s="14"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="24" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
@@ -1708,7 +1708,7 @@
       <c r="H46" s="14"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="25"/>
+      <c r="A47" s="24"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
@@ -1728,7 +1728,7 @@
       <c r="H47" s="14"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="25"/>
+      <c r="A48" s="24"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1802,17 +1802,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1838,7 +1838,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>77</v>
       </c>
       <c r="B1" s="35"/>

</xml_diff>

<commit_message>
-Elaboración del segundo Plan de Iteración - Transición.
-Completado de secciones de la Memoria del proyecto.

-Actualización del repositorio en general.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="95">
   <si>
     <t>DOCUMENTACIÓN - METODOLOGÍA DE DESARROLLO PSI</t>
   </si>
@@ -186,27 +186,6 @@
     <t>Reunión de Requerimientos</t>
   </si>
   <si>
-    <t xml:space="preserve">NOTA: Me guié de las plantillas.dotx que habiamos descargado el año pasado. Ya que la página PSI no funciona adecuadamente. </t>
-  </si>
-  <si>
-    <t>Los documentos que se piden en la planificacion del 2018 y que no se encuentran en las plantillas son el Modelo de componentes y Clases de Diseño.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lo que se pide en la planificacion del 2018 para el Final es lo siguiente: </t>
-  </si>
-  <si>
-    <t>*Presentacion de la aplicación funcionando (web y móvil)</t>
-  </si>
-  <si>
-    <t>*Todo el proyecto completo listo</t>
-  </si>
-  <si>
-    <t>*Manuales (usuario, instalacion, etc)</t>
-  </si>
-  <si>
-    <t>*Memoria del proyecto.</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -240,9 +219,6 @@
     <t>Prototipos de Interfaz</t>
   </si>
   <si>
-    <t xml:space="preserve">Los que estan resaltados en amarillo son los documentos que se piden en la planificacion del 2018 y por lo tanto, son obligatorios. </t>
-  </si>
-  <si>
     <t>Memoria del Proyecto</t>
   </si>
   <si>
@@ -322,6 +298,29 @@
   </si>
   <si>
     <t>En total se encuentran finalizados 21 de 21 Documentos de Especificación.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOTA:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Los documentos que se encuentran resaltados en amarillo se piden en la planificacion del año 2018 y por lo tanto, son obligatorios. </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -553,9 +552,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -563,27 +583,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -922,15 +921,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
@@ -940,27 +939,27 @@
       <c r="N1" s="11"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="30"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="10"/>
       <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="32"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="32"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="15" t="s">
         <v>6</v>
       </c>
@@ -974,169 +973,169 @@
       <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="24"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="24"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="24"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="24"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="24"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="24"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="24"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="4" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G12" s="23"/>
       <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="24"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1148,69 +1147,69 @@
       <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="25" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G14" s="23"/>
       <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="24"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G15" s="23"/>
       <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="24"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G16" s="23"/>
       <c r="H16" s="14"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="24"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
@@ -1222,27 +1221,27 @@
       <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="24"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="5" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G18" s="23"/>
       <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="24"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="5" t="s">
         <v>22</v>
       </c>
@@ -1254,7 +1253,7 @@
       <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="24"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="5" t="s">
         <v>23</v>
       </c>
@@ -1266,7 +1265,7 @@
       <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="24"/>
+      <c r="A21" s="25"/>
       <c r="B21" s="5" t="s">
         <v>24</v>
       </c>
@@ -1278,67 +1277,67 @@
       <c r="H21" s="14"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="24"/>
+      <c r="A22" s="25"/>
       <c r="B22" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G22" s="23"/>
       <c r="H22" s="14"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="24"/>
+      <c r="A23" s="25"/>
       <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G23" s="23"/>
       <c r="H23" s="14"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="24"/>
+      <c r="A24" s="25"/>
       <c r="B24" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G24" s="23"/>
       <c r="H24" s="14"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="24"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="5" t="s">
         <v>28</v>
       </c>
@@ -1350,7 +1349,7 @@
       <c r="H25" s="14"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="24"/>
+      <c r="A26" s="25"/>
       <c r="B26" s="5" t="s">
         <v>29</v>
       </c>
@@ -1362,7 +1361,7 @@
       <c r="H26" s="14"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="24"/>
+      <c r="A27" s="25"/>
       <c r="B27" s="6" t="s">
         <v>30</v>
       </c>
@@ -1374,7 +1373,7 @@
       <c r="H27" s="14"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="24"/>
+      <c r="A28" s="25"/>
       <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
@@ -1386,7 +1385,7 @@
       <c r="H28" s="14"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="24"/>
+      <c r="A29" s="25"/>
       <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
@@ -1398,87 +1397,87 @@
       <c r="H29" s="14"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="24"/>
+      <c r="A30" s="25"/>
       <c r="B30" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G30" s="23"/>
       <c r="H30" s="14"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="24"/>
+      <c r="A31" s="25"/>
       <c r="B31" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G31" s="23"/>
       <c r="H31" s="14"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="24"/>
+      <c r="A32" s="25"/>
       <c r="B32" s="5" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G32" s="23"/>
       <c r="H32" s="14"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="24"/>
+      <c r="A33" s="25"/>
       <c r="B33" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G33" s="23"/>
       <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="25" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="5" t="s">
@@ -1492,7 +1491,7 @@
       <c r="H34" s="14"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="24"/>
+      <c r="A35" s="25"/>
       <c r="B35" s="5" t="s">
         <v>39</v>
       </c>
@@ -1504,7 +1503,7 @@
       <c r="H35" s="14"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="24"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="5" t="s">
         <v>40</v>
       </c>
@@ -1516,83 +1515,83 @@
       <c r="H36" s="14"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="32" t="s">
         <v>41</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G37" s="23"/>
       <c r="H37" s="14"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="26"/>
+      <c r="A38" s="33"/>
       <c r="B38" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G38" s="23"/>
       <c r="H38" s="14"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="26"/>
+      <c r="A39" s="33"/>
       <c r="B39" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G39" s="23"/>
       <c r="H39" s="14"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="27"/>
+      <c r="A40" s="34"/>
       <c r="B40" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G40" s="23"/>
       <c r="H40" s="14"/>
@@ -1605,44 +1604,44 @@
         <v>46</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G41" s="23"/>
       <c r="H41" s="14"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="24" t="s">
+      <c r="A42" s="25" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G42" s="23"/>
       <c r="H42" s="14"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="24"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="5" t="s">
         <v>49</v>
       </c>
@@ -1654,7 +1653,7 @@
       <c r="H43" s="14"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="24"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
@@ -1666,69 +1665,69 @@
       <c r="H44" s="14"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="24"/>
+      <c r="A45" s="25"/>
       <c r="B45" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G45" s="23"/>
       <c r="H45" s="14"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="24" t="s">
+      <c r="A46" s="25" t="s">
         <v>52</v>
       </c>
       <c r="B46" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G46" s="23"/>
       <c r="H46" s="14"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="24"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="6" t="s">
         <v>54</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="G47" s="23"/>
       <c r="H47" s="14"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="24"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="5" t="s">
         <v>55</v>
       </c>
@@ -1744,45 +1743,12 @@
       <c r="H49" s="14"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="A50" t="s">
-        <v>57</v>
-      </c>
       <c r="G50" s="14"/>
       <c r="H50" s="14"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -1802,17 +1768,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1838,8 +1804,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="28" t="s">
-        <v>77</v>
+      <c r="A1" s="24" t="s">
+        <v>69</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -1857,7 +1823,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="36" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
@@ -1873,7 +1839,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="37" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B7" s="38" t="s">
         <v>4</v>
@@ -1890,301 +1856,301 @@
         <v>5</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:14">
       <c r="A11" s="3" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:14">
       <c r="A12" s="3" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:14">
       <c r="A13" s="3" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="3" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="3" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Actualización de secciones de la presentación final.
-Actualización y cierre del Seguimiento de Documentación.
</commit_message>
<xml_diff>
--- a/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
+++ b/Seguimiento del Sistema/Seguimiento Documentacion.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="95">
   <si>
     <t>DOCUMENTACIÓN - METODOLOGÍA DE DESARROLLO PSI</t>
   </si>
@@ -351,7 +351,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,6 +397,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,14 +499,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -555,9 +564,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -576,15 +582,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -596,6 +593,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -921,830 +936,958 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="22"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="21"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="29"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="15" t="s">
+      <c r="A4" s="27"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="22"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="21"/>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="34" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="14"/>
+      <c r="D5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="22"/>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="25"/>
-      <c r="B6" s="4" t="s">
+      <c r="A6" s="34"/>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="14"/>
+      <c r="D6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="22"/>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="25"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="34"/>
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="14"/>
+      <c r="D7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="22"/>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="25"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="34"/>
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="14"/>
+      <c r="D8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="22"/>
+      <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="25"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="34"/>
+      <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="14"/>
+      <c r="D9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="22"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="25"/>
-      <c r="B10" s="4" t="s">
+      <c r="A10" s="34"/>
+      <c r="B10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="14"/>
+      <c r="D10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="25"/>
-      <c r="B11" s="4" t="s">
+      <c r="A11" s="34"/>
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="14"/>
+      <c r="D11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="25"/>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="34"/>
+      <c r="B12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="14"/>
+      <c r="D12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="22"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="25"/>
+      <c r="A13" s="34"/>
       <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="14"/>
+      <c r="C13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="22"/>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="14"/>
+      <c r="D14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="25"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="35"/>
+      <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="14"/>
+      <c r="D15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="22"/>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="25"/>
-      <c r="B16" s="5" t="s">
+      <c r="A16" s="35"/>
+      <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="14"/>
+      <c r="D16" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="25"/>
-      <c r="B17" s="5" t="s">
+      <c r="A17" s="35"/>
+      <c r="B17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="14"/>
+      <c r="C17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="22"/>
+      <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="25"/>
-      <c r="B18" s="5" t="s">
+      <c r="A18" s="35"/>
+      <c r="B18" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="23"/>
-      <c r="H18" s="14"/>
+      <c r="D18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="22"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="25"/>
-      <c r="B19" s="5" t="s">
+      <c r="A19" s="35"/>
+      <c r="B19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="14"/>
+      <c r="C19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="22"/>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="25"/>
-      <c r="B20" s="5" t="s">
+      <c r="A20" s="35"/>
+      <c r="B20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="14"/>
+      <c r="C20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="22"/>
+      <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="25"/>
-      <c r="B21" s="5" t="s">
+      <c r="A21" s="35"/>
+      <c r="B21" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="14"/>
+      <c r="C21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="22"/>
+      <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="25"/>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="35"/>
+      <c r="B22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G22" s="23"/>
-      <c r="H22" s="14"/>
+      <c r="D22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="22"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="25"/>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="35"/>
+      <c r="B23" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="14"/>
+      <c r="D23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="22"/>
+      <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8">
-      <c r="A24" s="25"/>
-      <c r="B24" s="6" t="s">
+      <c r="A24" s="35"/>
+      <c r="B24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="14"/>
+      <c r="D24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="22"/>
+      <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8">
-      <c r="A25" s="25"/>
-      <c r="B25" s="5" t="s">
+      <c r="A25" s="35"/>
+      <c r="B25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="14"/>
+      <c r="C25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="22"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8">
-      <c r="A26" s="25"/>
-      <c r="B26" s="5" t="s">
+      <c r="A26" s="35"/>
+      <c r="B26" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="14"/>
+      <c r="C26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="22"/>
+      <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8">
-      <c r="A27" s="25"/>
-      <c r="B27" s="6" t="s">
+      <c r="A27" s="35"/>
+      <c r="B27" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="14"/>
+      <c r="C27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="22"/>
+      <c r="H27" s="13"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="25"/>
-      <c r="B28" s="6" t="s">
+      <c r="A28" s="35"/>
+      <c r="B28" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="14"/>
+      <c r="C28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="22"/>
+      <c r="H28" s="13"/>
     </row>
     <row r="29" spans="1:8">
-      <c r="A29" s="25"/>
-      <c r="B29" s="6" t="s">
+      <c r="A29" s="35"/>
+      <c r="B29" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="14"/>
+      <c r="C29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="22"/>
+      <c r="H29" s="13"/>
     </row>
     <row r="30" spans="1:8">
-      <c r="A30" s="25"/>
-      <c r="B30" s="4" t="s">
+      <c r="A30" s="35"/>
+      <c r="B30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G30" s="23"/>
-      <c r="H30" s="14"/>
+      <c r="D30" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="22"/>
+      <c r="H30" s="13"/>
     </row>
     <row r="31" spans="1:8">
-      <c r="A31" s="25"/>
-      <c r="B31" s="4" t="s">
+      <c r="A31" s="35"/>
+      <c r="B31" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G31" s="23"/>
-      <c r="H31" s="14"/>
+      <c r="D31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="22"/>
+      <c r="H31" s="13"/>
     </row>
     <row r="32" spans="1:8">
-      <c r="A32" s="25"/>
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="35"/>
+      <c r="B32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G32" s="23"/>
-      <c r="H32" s="14"/>
+      <c r="D32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="22"/>
+      <c r="H32" s="13"/>
     </row>
     <row r="33" spans="1:8">
-      <c r="A33" s="25"/>
-      <c r="B33" s="4" t="s">
+      <c r="A33" s="35"/>
+      <c r="B33" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G33" s="23"/>
-      <c r="H33" s="14"/>
+      <c r="D33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" s="22"/>
+      <c r="H33" s="13"/>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="14"/>
+      <c r="C34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" s="22"/>
+      <c r="H34" s="13"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="25"/>
-      <c r="B35" s="5" t="s">
+      <c r="A35" s="34"/>
+      <c r="B35" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="14"/>
+      <c r="C35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="22"/>
+      <c r="H35" s="13"/>
     </row>
     <row r="36" spans="1:8">
-      <c r="A36" s="25"/>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="34"/>
+      <c r="B36" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="14"/>
+      <c r="C36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" s="22"/>
+      <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="32" t="s">
+      <c r="A37" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D37" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F37" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="G37" s="23"/>
-      <c r="H37" s="14"/>
+      <c r="D37" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F37" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="22"/>
+      <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:8">
-      <c r="A38" s="33"/>
-      <c r="B38" s="5" t="s">
+      <c r="A38" s="37"/>
+      <c r="B38" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G38" s="23"/>
-      <c r="H38" s="14"/>
+      <c r="D38" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G38" s="22"/>
+      <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8">
-      <c r="A39" s="33"/>
-      <c r="B39" s="4" t="s">
+      <c r="A39" s="37"/>
+      <c r="B39" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F39" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G39" s="23"/>
-      <c r="H39" s="14"/>
+      <c r="D39" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39" s="22"/>
+      <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:8">
-      <c r="A40" s="34"/>
-      <c r="B40" s="4" t="s">
+      <c r="A40" s="38"/>
+      <c r="B40" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G40" s="23"/>
-      <c r="H40" s="14"/>
+      <c r="D40" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G40" s="22"/>
+      <c r="H40" s="13"/>
     </row>
     <row r="41" spans="1:8">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F41" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G41" s="23"/>
-      <c r="H41" s="14"/>
+      <c r="D41" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G41" s="22"/>
+      <c r="H41" s="13"/>
     </row>
     <row r="42" spans="1:8">
-      <c r="A42" s="25" t="s">
+      <c r="A42" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F42" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G42" s="23"/>
-      <c r="H42" s="14"/>
+      <c r="D42" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G42" s="22"/>
+      <c r="H42" s="13"/>
     </row>
     <row r="43" spans="1:8">
-      <c r="A43" s="25"/>
-      <c r="B43" s="5" t="s">
+      <c r="A43" s="35"/>
+      <c r="B43" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="14"/>
+      <c r="C43" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G43" s="22"/>
+      <c r="H43" s="13"/>
     </row>
     <row r="44" spans="1:8">
-      <c r="A44" s="25"/>
-      <c r="B44" s="5" t="s">
+      <c r="A44" s="35"/>
+      <c r="B44" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="14"/>
+      <c r="C44" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G44" s="22"/>
+      <c r="H44" s="13"/>
     </row>
     <row r="45" spans="1:8">
-      <c r="A45" s="25"/>
-      <c r="B45" s="4" t="s">
+      <c r="A45" s="35"/>
+      <c r="B45" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G45" s="23"/>
-      <c r="H45" s="14"/>
+      <c r="D45" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G45" s="22"/>
+      <c r="H45" s="13"/>
     </row>
     <row r="46" spans="1:8">
-      <c r="A46" s="25" t="s">
+      <c r="A46" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G46" s="23"/>
-      <c r="H46" s="14"/>
+      <c r="D46" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G46" s="22"/>
+      <c r="H46" s="13"/>
     </row>
     <row r="47" spans="1:8">
-      <c r="A47" s="25"/>
-      <c r="B47" s="6" t="s">
+      <c r="A47" s="34"/>
+      <c r="B47" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F47" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G47" s="23"/>
-      <c r="H47" s="14"/>
+      <c r="D47" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G47" s="22"/>
+      <c r="H47" s="13"/>
     </row>
     <row r="48" spans="1:8">
-      <c r="A48" s="25"/>
-      <c r="B48" s="5" t="s">
+      <c r="A48" s="34"/>
+      <c r="B48" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="23"/>
-      <c r="H48" s="14"/>
+      <c r="C48" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G48" s="22"/>
+      <c r="H48" s="13"/>
     </row>
     <row r="49" spans="1:8">
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
     </row>
     <row r="50" spans="1:8">
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
@@ -1752,33 +1895,33 @@
       </c>
     </row>
     <row r="63" spans="1:8">
-      <c r="A63" s="8"/>
+      <c r="A63" s="7"/>
     </row>
     <row r="64" spans="1:8">
-      <c r="A64" s="8"/>
+      <c r="A64" s="7"/>
     </row>
     <row r="66" spans="1:1">
-      <c r="A66" s="8"/>
+      <c r="A66" s="7"/>
     </row>
     <row r="68" spans="1:1">
-      <c r="A68" s="8"/>
+      <c r="A68" s="7"/>
     </row>
     <row r="69" spans="1:1">
-      <c r="A69" s="8"/>
+      <c r="A69" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A14:A33"/>
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="A37:A40"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A5:A13"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A14:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="A37:A40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -1804,352 +1947,352 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="37"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="B9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:14">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="B11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="B12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="B14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:14">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="3" t="s">
+      <c r="B15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:14">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="B16" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="B17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="B18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="B19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="3" t="s">
+      <c r="B20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="3" t="s">
+      <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="B22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="3" t="s">
+      <c r="B23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="B24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="3" t="s">
+      <c r="B25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="B26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="3" t="s">
+      <c r="B27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="B28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>